<commit_message>
Se organizaron los archivos en la carpeta src
</commit_message>
<xml_diff>
--- a/Mercado Liebre - Entregable.xlsx
+++ b/Mercado Liebre - Entregable.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\digital-house\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\digital-house\mercado-liebre-entregable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF85495B-E5C8-4AC2-9405-368EE5C0B2AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0F585D-472D-47FF-AA17-C7596BC7998D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="103">
   <si>
     <t>REQUERIDOS</t>
   </si>
@@ -398,6 +398,9 @@
   </si>
   <si>
     <t>! Donde se guarda?</t>
+  </si>
+  <si>
+    <t>Crear campo de foto</t>
   </si>
 </sst>
 </file>
@@ -809,8 +812,8 @@
   </sheetPr>
   <dimension ref="A1:Z1047"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:E40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3475,7 +3478,9 @@
         <v>101</v>
       </c>
       <c r="G74" s="8"/>
-      <c r="H74" s="8"/>
+      <c r="H74" s="8" t="s">
+        <v>102</v>
+      </c>
       <c r="I74" s="8"/>
       <c r="J74" s="8"/>
       <c r="K74" s="8"/>

</xml_diff>

<commit_message>
Al crear un producto se redirige al detalle del mismo
</commit_message>
<xml_diff>
--- a/Mercado Liebre - Entregable.xlsx
+++ b/Mercado Liebre - Entregable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\digital-house\mercado-liebre-entregable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0F585D-472D-47FF-AA17-C7596BC7998D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0664928-F617-46BC-AAA8-F0A3A9744898}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -812,8 +812,8 @@
   </sheetPr>
   <dimension ref="A1:Z1047"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:E25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1814,17 +1814,17 @@
       <c r="Z27" s="8"/>
     </row>
     <row r="28" spans="1:26">
-      <c r="A28" s="22"/>
-      <c r="B28" s="23" t="s">
+      <c r="A28" s="15"/>
+      <c r="B28" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28" s="17">
         <v>1</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="24">
+      <c r="E28" s="17">
         <v>1</v>
       </c>
       <c r="F28" s="8"/>

</xml_diff>

<commit_message>
Ahora si el formulario da error los datos ingresados quedan
</commit_message>
<xml_diff>
--- a/Mercado Liebre - Entregable.xlsx
+++ b/Mercado Liebre - Entregable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\digital-house\mercado-liebre-entregable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0664928-F617-46BC-AAA8-F0A3A9744898}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E6B80D-BE4E-4A3C-B710-92597C97692E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="103">
   <si>
     <t>REQUERIDOS</t>
   </si>
@@ -812,8 +812,8 @@
   </sheetPr>
   <dimension ref="A1:Z1047"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:E28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1740,22 +1740,20 @@
       <c r="Z25" s="8"/>
     </row>
     <row r="26" spans="1:26">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23" t="s">
+      <c r="A26" s="15"/>
+      <c r="B26" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="17">
         <v>2</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E26" s="17">
         <v>2</v>
       </c>
-      <c r="F26" s="8" t="s">
-        <v>100</v>
-      </c>
+      <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>

</xml_diff>

<commit_message>
La categoria no es editable en la edicion de productos
</commit_message>
<xml_diff>
--- a/Mercado Liebre - Entregable.xlsx
+++ b/Mercado Liebre - Entregable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\digital-house\mercado-liebre-entregable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E6B80D-BE4E-4A3C-B710-92597C97692E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29ABA69-1382-4416-AFC3-994932C4AF2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="103">
   <si>
     <t>REQUERIDOS</t>
   </si>
@@ -812,8 +812,8 @@
   </sheetPr>
   <dimension ref="A1:Z1047"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2068,22 +2068,20 @@
       <c r="Z34" s="8"/>
     </row>
     <row r="35" spans="1:26">
-      <c r="A35" s="22"/>
-      <c r="B35" s="23" t="s">
+      <c r="A35" s="15"/>
+      <c r="B35" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="24">
+      <c r="C35" s="17">
         <v>1</v>
       </c>
-      <c r="D35" s="23" t="s">
+      <c r="D35" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="24">
+      <c r="E35" s="17">
         <v>2</v>
       </c>
-      <c r="F35" s="8" t="s">
-        <v>98</v>
-      </c>
+      <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>

</xml_diff>

<commit_message>
Los campos del login quedan completos en caso de error
</commit_message>
<xml_diff>
--- a/Mercado Liebre - Entregable.xlsx
+++ b/Mercado Liebre - Entregable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\digital-house\mercado-liebre-entregable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29ABA69-1382-4416-AFC3-994932C4AF2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A4EC1E-FF8D-452A-8C9A-F544389B463F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="102">
   <si>
     <t>REQUERIDOS</t>
   </si>
@@ -394,9 +394,6 @@
     <t>Ver como mostrar el error</t>
   </si>
   <si>
-    <t>!</t>
-  </si>
-  <si>
     <t>! Donde se guarda?</t>
   </si>
   <si>
@@ -585,12 +582,12 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -812,8 +809,8 @@
   </sheetPr>
   <dimension ref="A1:Z1047"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2249,7 +2246,7 @@
     </row>
     <row r="40" spans="1:26">
       <c r="A40" s="25"/>
-      <c r="B40" s="34" t="s">
+      <c r="B40" s="31" t="s">
         <v>49</v>
       </c>
       <c r="C40" s="24">
@@ -2612,22 +2609,20 @@
       <c r="Z49" s="8"/>
     </row>
     <row r="50" spans="1:26">
-      <c r="A50" s="25"/>
-      <c r="B50" s="23" t="s">
+      <c r="A50" s="19"/>
+      <c r="B50" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C50" s="24">
+      <c r="C50" s="17">
         <v>1</v>
       </c>
-      <c r="D50" s="23" t="s">
+      <c r="D50" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E50" s="24">
+      <c r="E50" s="17">
         <v>2</v>
       </c>
-      <c r="F50" s="8" t="s">
-        <v>100</v>
-      </c>
+      <c r="F50" s="8"/>
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
@@ -2832,22 +2827,20 @@
       <c r="Z55" s="8"/>
     </row>
     <row r="56" spans="1:26">
-      <c r="A56" s="31"/>
-      <c r="B56" s="32" t="s">
+      <c r="A56" s="32"/>
+      <c r="B56" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C56" s="33">
+      <c r="C56" s="34">
         <v>1</v>
       </c>
-      <c r="D56" s="32" t="s">
+      <c r="D56" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E56" s="33">
+      <c r="E56" s="34">
         <v>2</v>
       </c>
-      <c r="F56" s="8" t="s">
-        <v>100</v>
-      </c>
+      <c r="F56" s="8"/>
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
       <c r="I56" s="8"/>
@@ -3471,11 +3464,11 @@
         <v>1</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G74" s="8"/>
       <c r="H74" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I74" s="8"/>
       <c r="J74" s="8"/>

</xml_diff>

<commit_message>
Se modifico la apariencia de los errores
</commit_message>
<xml_diff>
--- a/Mercado Liebre - Entregable.xlsx
+++ b/Mercado Liebre - Entregable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\digital-house\mercado-liebre-entregable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A4EC1E-FF8D-452A-8C9A-F544389B463F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F63AF9-BAD5-4577-A4F1-0DF12BC6F57E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="103">
   <si>
     <t>REQUERIDOS</t>
   </si>
@@ -398,6 +398,9 @@
   </si>
   <si>
     <t>Crear campo de foto</t>
+  </si>
+  <si>
+    <t>Como hacer para primero mostrar los values del producto a editar?</t>
   </si>
 </sst>
 </file>
@@ -809,8 +812,8 @@
   </sheetPr>
   <dimension ref="A1:Z1047"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2330,7 +2333,9 @@
       <c r="E42" s="24">
         <v>2</v>
       </c>
-      <c r="F42" s="8"/>
+      <c r="F42" s="8" t="s">
+        <v>102</v>
+      </c>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>

</xml_diff>

<commit_message>
Intentando que en caso de error no se borren los campos del form de edicion
</commit_message>
<xml_diff>
--- a/Mercado Liebre - Entregable.xlsx
+++ b/Mercado Liebre - Entregable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\digital-house\mercado-liebre-entregable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F63AF9-BAD5-4577-A4F1-0DF12BC6F57E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08512B9E-1382-439F-8703-FF8678145786}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -812,7 +812,7 @@
   </sheetPr>
   <dimension ref="A1:Z1047"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Las validaciones aparecen junto al campo en la creacion de producto
</commit_message>
<xml_diff>
--- a/Mercado Liebre - Entregable.xlsx
+++ b/Mercado Liebre - Entregable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\digital-house\mercado-liebre-entregable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08512B9E-1382-439F-8703-FF8678145786}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65535BD3-175A-44E3-AA5E-3AAA85739328}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -812,8 +812,8 @@
   </sheetPr>
   <dimension ref="A1:Z1047"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1666,17 +1666,17 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" spans="1:26">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23" t="s">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="17">
         <v>2</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="D24" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="17">
         <v>4</v>
       </c>
       <c r="F24" s="8"/>

</xml_diff>

<commit_message>
Se encontro un bug en las validaciones y se volvio a la version anteriror
</commit_message>
<xml_diff>
--- a/Mercado Liebre - Entregable.xlsx
+++ b/Mercado Liebre - Entregable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\digital-house\mercado-liebre-entregable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65535BD3-175A-44E3-AA5E-3AAA85739328}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0215838-B056-4C15-BA53-4B8A771DCEBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -812,7 +812,7 @@
   </sheetPr>
   <dimension ref="A1:Z1047"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A24" sqref="A24:E24"/>
     </sheetView>
   </sheetViews>
@@ -1666,17 +1666,17 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" spans="1:26">
-      <c r="A24" s="15"/>
-      <c r="B24" s="16" t="s">
+      <c r="A24" s="22"/>
+      <c r="B24" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="24">
         <v>2</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="24">
         <v>4</v>
       </c>
       <c r="F24" s="8"/>

</xml_diff>

<commit_message>
Se retoco el input de stock en la edicion y creacion de productos
</commit_message>
<xml_diff>
--- a/Mercado Liebre - Entregable.xlsx
+++ b/Mercado Liebre - Entregable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\digital-house\mercado-liebre-entregable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0215838-B056-4C15-BA53-4B8A771DCEBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EA2B04-4822-427B-99BD-1FA514C52E0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="102">
   <si>
     <t>REQUERIDOS</t>
   </si>
@@ -398,9 +398,6 @@
   </si>
   <si>
     <t>Crear campo de foto</t>
-  </si>
-  <si>
-    <t>Como hacer para primero mostrar los values del producto a editar?</t>
   </si>
 </sst>
 </file>
@@ -812,8 +809,8 @@
   </sheetPr>
   <dimension ref="A1:Z1047"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:E24"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2320,22 +2317,20 @@
       <c r="Z41" s="8"/>
     </row>
     <row r="42" spans="1:26">
-      <c r="A42" s="22"/>
-      <c r="B42" s="23" t="s">
+      <c r="A42" s="15"/>
+      <c r="B42" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="24">
+      <c r="C42" s="17">
         <v>2</v>
       </c>
-      <c r="D42" s="23" t="s">
+      <c r="D42" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="24">
+      <c r="E42" s="17">
         <v>2</v>
       </c>
-      <c r="F42" s="8" t="s">
-        <v>102</v>
-      </c>
+      <c r="F42" s="8"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>

</xml_diff>

<commit_message>
Cambio de imagen opcional, si no cambia mantiene la anterior
</commit_message>
<xml_diff>
--- a/Mercado Liebre - Entregable.xlsx
+++ b/Mercado Liebre - Entregable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\digital-house\mercado-liebre-entregable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EA2B04-4822-427B-99BD-1FA514C52E0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B685FE3D-FE66-4CC0-B2B6-5731943983DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="103">
   <si>
     <t>REQUERIDOS</t>
   </si>
@@ -399,6 +399,9 @@
   <si>
     <t>Crear campo de foto</t>
   </si>
+  <si>
+    <t>La imagen se sube igual aunque no valide el form en otros campos</t>
+  </si>
 </sst>
 </file>
 
@@ -462,7 +465,7 @@
       <name val="Nunito"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -510,12 +513,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -530,7 +527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -582,7 +579,6 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -809,8 +805,8 @@
   </sheetPr>
   <dimension ref="A1:Z1047"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:E59"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2245,20 +2241,22 @@
       <c r="Z39" s="8"/>
     </row>
     <row r="40" spans="1:26">
-      <c r="A40" s="25"/>
-      <c r="B40" s="31" t="s">
+      <c r="A40" s="19"/>
+      <c r="B40" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="24">
+      <c r="C40" s="17">
         <v>2</v>
       </c>
-      <c r="D40" s="23" t="s">
+      <c r="D40" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E40" s="24">
+      <c r="E40" s="17">
         <v>2</v>
       </c>
-      <c r="F40" s="8"/>
+      <c r="F40" s="8" t="s">
+        <v>102</v>
+      </c>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
@@ -2827,17 +2825,17 @@
       <c r="Z55" s="8"/>
     </row>
     <row r="56" spans="1:26">
-      <c r="A56" s="32"/>
-      <c r="B56" s="33" t="s">
+      <c r="A56" s="31"/>
+      <c r="B56" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C56" s="34">
+      <c r="C56" s="33">
         <v>1</v>
       </c>
-      <c r="D56" s="33" t="s">
+      <c r="D56" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="E56" s="34">
+      <c r="E56" s="33">
         <v>2</v>
       </c>
       <c r="F56" s="8"/>

</xml_diff>

<commit_message>
Campo de avatar para los usuarios e imagen generica seteda
</commit_message>
<xml_diff>
--- a/Mercado Liebre - Entregable.xlsx
+++ b/Mercado Liebre - Entregable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\digital-house\mercado-liebre-entregable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B685FE3D-FE66-4CC0-B2B6-5731943983DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C044800-3771-4EA6-8747-B5302DCA4978}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -805,8 +805,8 @@
   </sheetPr>
   <dimension ref="A1:Z1047"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Es posible cambiar el avatar del usuario
</commit_message>
<xml_diff>
--- a/Mercado Liebre - Entregable.xlsx
+++ b/Mercado Liebre - Entregable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\digital-house\mercado-liebre-entregable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C044800-3771-4EA6-8747-B5302DCA4978}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C435135-7EFA-4951-AC7B-A6222D8541D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="102">
   <si>
     <t>REQUERIDOS</t>
   </si>
@@ -394,13 +394,10 @@
     <t>Ver como mostrar el error</t>
   </si>
   <si>
-    <t>! Donde se guarda?</t>
+    <t>La imagen se sube igual aunque no valide el form en otros campos</t>
   </si>
   <si>
-    <t>Crear campo de foto</t>
-  </si>
-  <si>
-    <t>La imagen se sube igual aunque no valide el form en otros campos</t>
+    <t>El cambio se hace cuando se desloguea y vuelve a loguear</t>
   </si>
 </sst>
 </file>
@@ -805,8 +802,8 @@
   </sheetPr>
   <dimension ref="A1:Z1047"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2255,7 +2252,7 @@
         <v>2</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
@@ -3448,26 +3445,24 @@
       <c r="Z73" s="8"/>
     </row>
     <row r="74" spans="1:26">
-      <c r="A74" s="25"/>
-      <c r="B74" s="23" t="s">
+      <c r="A74" s="19"/>
+      <c r="B74" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C74" s="24">
+      <c r="C74" s="17">
         <v>1</v>
       </c>
-      <c r="D74" s="23" t="s">
+      <c r="D74" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E74" s="24">
+      <c r="E74" s="17">
         <v>1</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G74" s="8"/>
-      <c r="H74" s="8" t="s">
-        <v>101</v>
-      </c>
+      <c r="H74" s="8"/>
       <c r="I74" s="8"/>
       <c r="J74" s="8"/>
       <c r="K74" s="8"/>

</xml_diff>